<commit_message>
Actualización 4 de julio de 2023 - Lap HP
Se actualiza el repositorio con material del curso de Física 2
</commit_message>
<xml_diff>
--- a/Combinacion/Concentrado_Actividades_Fisica_2_263.xlsx
+++ b/Combinacion/Concentrado_Actividades_Fisica_2_263.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Cuatrimestral\Fisica_2_BC\Combinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E35235-EB23-4A5F-B89B-9D4FCDAA8DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3726115-0923-42D8-A18C-A47E84FC026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A9CAC45-FC4B-4108-A13C-1EA279EAC0D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Analisis_1Parcial" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Analisis_1Parcial!$R$2:$R$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Analisis_1Parcial!$S$2:$S$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="197">
   <si>
     <t>Matrícula</t>
   </si>
@@ -588,6 +615,45 @@
   </si>
   <si>
     <t>Primer_Parcial</t>
+  </si>
+  <si>
+    <t>Acreditación</t>
+  </si>
+  <si>
+    <t>Acredita</t>
+  </si>
+  <si>
+    <t>No Acredita</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>&lt; 6</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>6 -7</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>7 - 8</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>8 - 9</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>9 -10</t>
   </si>
 </sst>
 </file>
@@ -664,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,6 +755,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,6 +774,1904 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX" sz="2000">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Porcentaje</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" sz="2000" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> de acreditación</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-CE04-4A79-ABE1-779AA92EAE61}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CE04-4A79-ABE1-779AA92EAE61}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4865704286964128E-2"/>
+                  <c:y val="-6.6185476815398079E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-CE04-4A79-ABE1-779AA92EAE61}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.2506561679790026E-2"/>
+                  <c:y val="-3.3549868766404117E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-CE04-4A79-ABE1-779AA92EAE61}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analisis_1Parcial!$E$2:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No Acredita</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Acredita</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analisis_1Parcial!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE04-4A79-ABE1-779AA92EAE61}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Calificaciones del examen</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analisis_1Parcial!$R$2:$R$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>&lt; 6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6 -7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7 - 8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 - 9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9 -10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analisis_1Parcial!$S$2:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C57-4726-8C44-FA78E6D85408}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="16"/>
+        <c:axId val="2044387056"/>
+        <c:axId val="1627120416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2044387056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1627120416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1627120416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2044387056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F0A454-4C08-F429-5FB9-86952EB3C8A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B6B651E-E222-F4D8-C858-DF59DEC0989A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1005,11 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42643DA-6EB3-45A9-9EC3-04F699E09DA9}">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7395" ySplit="600" topLeftCell="J31" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3906,4 +5871,790 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F626EA-F489-4DA9-82A9-403689CF24D8}">
+  <dimension ref="A1:S47"/>
+  <sheetViews>
+    <sheetView topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="15" max="15" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>7.2166666666666659</v>
+      </c>
+      <c r="C2" s="1" cm="1">
+        <f t="array" ref="C2:C47">IF(A2:A47&lt;6,1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(C2:C47,"=1")</f>
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>IF(AND(N2&gt;=6,N2&lt;7),"B",IF(AND(N2&gt;=7,N2&lt;8),"C",IF(AND(N2&gt;=8,N2&lt;9),"D",IF(AND(N2&gt;=9,N2&lt;=10),"E","A"))))</f>
+        <v>C</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="S2">
+        <f>COUNTIF($O$2:$O$47,"=A")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>8.3083333333333318</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(C2:C47,"=2")</f>
+        <v>35</v>
+      </c>
+      <c r="N3" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" ref="O3:O47" si="0">IF(AND(N3&gt;=6,N3&lt;7),"B",IF(AND(N3&gt;=7,N3&lt;8),"C",IF(AND(N3&gt;=8,N3&lt;9),"D",IF(AND(N3&gt;=9,N3&lt;=10),"E","A"))))</f>
+        <v>D</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="S3">
+        <f>COUNTIF($O$2:$O$47,"=B")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2.5277777777777777</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="S4">
+        <f>COUNTIF($O$2:$O$47,"=C")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>7.4111111111111105</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="S5">
+        <f>COUNTIF($O$2:$O$476,"=D")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>8.9888888888888872</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>8</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="S6">
+        <f>COUNTIF($O$2:$O$47,"=E")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>9.3583333333333325</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>9.1083333333333325</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7.6138888888888889</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>7.4416666666666655</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>6.7138888888888886</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>8.7333333333333307</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>8</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>8.0694444444444446</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>7.197222222222222</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>7.2916666666666661</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>7</v>
+      </c>
+      <c r="O15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>8.0555555555555554</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="N16" s="2">
+        <v>7</v>
+      </c>
+      <c r="O16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>8.9944444444444454</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>9</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>8.0888888888888886</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>9</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>7.3805555555555555</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="N20" s="2">
+        <v>7</v>
+      </c>
+      <c r="O20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>9.1888888888888882</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="N21" s="2">
+        <v>9</v>
+      </c>
+      <c r="O21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>8.4805555555555543</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="N22" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>5.2638888888888884</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>9.0333333333333314</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>8</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>6.3166666666666655</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="N26" s="2">
+        <v>7</v>
+      </c>
+      <c r="O26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>6.7666666666666666</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2">
+        <v>8</v>
+      </c>
+      <c r="O27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>5.1333333333333329</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="2">
+        <v>8</v>
+      </c>
+      <c r="O28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>4.4388888888888882</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>9</v>
+      </c>
+      <c r="O29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="O30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>5.6833333333333336</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="O31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>7.333333333333333</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="N32" s="2">
+        <v>4</v>
+      </c>
+      <c r="O32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>5.2305555555555552</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>7.43611111111111</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="N34" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>6.0416666666666661</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="N35" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>2.8388888888888886</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="N36" s="2">
+        <v>7</v>
+      </c>
+      <c r="O36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>8.68611111111111</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="N37" s="2">
+        <v>9</v>
+      </c>
+      <c r="O37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>7.7381250000000001</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="N38" s="2">
+        <v>9</v>
+      </c>
+      <c r="O38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>7.1916666666666664</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="N39" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="O39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>8.2833333333333314</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="N40" s="2">
+        <v>8</v>
+      </c>
+      <c r="O40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>1.9249999999999998</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="N41" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="O41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>8.2583333333333329</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="N42" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="O42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>6.3666666666666654</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="N43" s="2">
+        <v>8</v>
+      </c>
+      <c r="O43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>8.6694444444444443</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="N44" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>9.2833333333333314</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="N45" s="2">
+        <v>10</v>
+      </c>
+      <c r="O45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>8.81111111111111</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="N46" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="O46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>8.0833333333333321</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="N47" s="2">
+        <v>7</v>
+      </c>
+      <c r="O47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>